<commit_message>
Fix same action in one node
</commit_message>
<xml_diff>
--- a/sources/Pattern.xlsx
+++ b/sources/Pattern.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergey Kharchenko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\GridPatternEA\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t>Gate0</t>
   </si>
@@ -263,6 +263,31 @@
   </si>
   <si>
     <r>
+      <t>BX1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BX2</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
@@ -282,18 +307,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> BX1</t>
+      <t/>
     </r>
   </si>
 </sst>
@@ -301,7 +315,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -480,6 +494,13 @@
       <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1026,6 +1047,33 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1035,21 +1083,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1057,18 +1090,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1395,7 +1416,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="F10" sqref="F10:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,25 +1467,25 @@
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="27">
         <v>10</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="27">
         <v>20</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="27">
         <v>10</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="18" t="s">
         <v>24</v>
       </c>
       <c r="I2" s="1">
@@ -1478,13 +1499,13 @@
       <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="21"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="15"/>
       <c r="I3" s="2">
         <v>-20</v>
       </c>
@@ -1496,15 +1517,15 @@
       <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="18">
+      <c r="B4" s="25"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="20">
         <v>-10</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I4" s="1">
@@ -1518,13 +1539,13 @@
       <c r="A5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="16"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="21"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="15"/>
       <c r="I5" s="2">
         <v>-30</v>
       </c>
@@ -1536,19 +1557,19 @@
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="18">
+      <c r="B6" s="25"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="20">
         <v>-20</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="28">
         <v>20</v>
       </c>
-      <c r="H6" s="29" t="s">
+      <c r="H6" s="19" t="s">
         <v>31</v>
       </c>
       <c r="I6" s="1">
@@ -1562,13 +1583,13 @@
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="21"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="2">
         <v>-20</v>
       </c>
@@ -1580,15 +1601,15 @@
       <c r="A8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="18">
+      <c r="B8" s="25"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="20">
         <v>-20</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="16" t="s">
         <v>30</v>
       </c>
       <c r="I8" s="1">
@@ -1602,13 +1623,13 @@
       <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="28"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="2">
         <v>-10</v>
       </c>
@@ -1620,43 +1641,43 @@
       <c r="A10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="18">
+      <c r="B10" s="25"/>
+      <c r="C10" s="20">
         <v>-10</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="24">
+      <c r="D10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="28">
         <v>30</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="28">
         <v>20</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I10" s="1">
         <v>10</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="21"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="15"/>
       <c r="I11" s="2">
         <v>-10</v>
       </c>
@@ -1668,15 +1689,15 @@
       <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="18">
+      <c r="B12" s="25"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="20">
         <v>-20</v>
       </c>
-      <c r="H12" s="21" t="s">
+      <c r="H12" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I12" s="1">
@@ -1690,13 +1711,13 @@
       <c r="A13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="21"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="15"/>
       <c r="I13" s="2">
         <v>-20</v>
       </c>
@@ -1708,19 +1729,19 @@
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="18">
+      <c r="B14" s="25"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="20">
         <v>-30</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="24">
+      <c r="G14" s="28">
         <v>10</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="16" t="s">
         <v>29</v>
       </c>
       <c r="I14" s="1">
@@ -1734,13 +1755,13 @@
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="28"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="16"/>
       <c r="I15" s="2">
         <v>-30</v>
       </c>
@@ -1752,15 +1773,15 @@
       <c r="A16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="18">
+      <c r="B16" s="25"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="20">
         <v>-10</v>
       </c>
-      <c r="H16" s="21" t="s">
+      <c r="H16" s="15" t="s">
         <v>24</v>
       </c>
       <c r="I16" s="1">
@@ -1774,13 +1795,13 @@
       <c r="A17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="22"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="17"/>
       <c r="I17" s="4">
         <v>-20</v>
       </c>
@@ -1790,19 +1811,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="E14:E17"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="F6:F9"/>
-    <mergeCell ref="F10:F13"/>
-    <mergeCell ref="F14:F17"/>
     <mergeCell ref="B2:B17"/>
     <mergeCell ref="C10:C17"/>
     <mergeCell ref="D10:D17"/>
@@ -1819,6 +1827,19 @@
     <mergeCell ref="E2:E5"/>
     <mergeCell ref="E6:E9"/>
     <mergeCell ref="E10:E13"/>
+    <mergeCell ref="E14:E17"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="F6:F9"/>
+    <mergeCell ref="F10:F13"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="H10:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>